<commit_message>
exel test (add after closing the file)
</commit_message>
<xml_diff>
--- a/דרישות ומקרי משתמש.xlsx
+++ b/דרישות ומקרי משתמש.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>נוסח</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>UC</t>
+  </si>
+  <si>
+    <t>ffffff</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -522,7 +525,9 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
exel test2 (cann't see change on gitHub)
</commit_message>
<xml_diff>
--- a/דרישות ומקרי משתמש.xlsx
+++ b/דרישות ומקרי משתמש.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>נוסח</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>UC</t>
-  </si>
-  <si>
-    <t>ffffff</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -525,9 +522,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>